<commit_message>
Auto-committed on 2023/10/06 週五 16:50:16.92
</commit_message>
<xml_diff>
--- a/Program/Other/L5735K_底稿_公會報送-保險業投資不動產及放款情形.xlsx
+++ b/Program/Other/L5735K_底稿_公會報送-保險業投資不動產及放款情形.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v06v2\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A20DD8-72B7-4E87-B15E-A02780444C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5620D1FF-B3F7-4D2E-843D-655145038EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="931" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -850,7 +850,7 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -871,12 +871,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="43"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -884,12 +878,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1066,14 +1054,8 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="36">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -1351,19 +1333,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1404,15 +1373,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1522,6 +1482,89 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1542,143 +1585,134 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="11" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="12" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="12" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="13" borderId="33" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="9" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="10" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="10" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="11" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="34" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="32" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -1688,7 +1722,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1">
@@ -1703,85 +1737,73 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="17" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="10" fontId="17" fillId="0" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="17" fillId="0" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="17" fillId="0" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="17" fillId="0" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="17" fillId="0" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="17" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="17" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1793,9 +1815,6 @@
     <xf numFmtId="180" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="17" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="17" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1805,13 +1824,13 @@
     <xf numFmtId="178" fontId="17" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1">
@@ -1823,22 +1842,76 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="14" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="28" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="44" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="17" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="22" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="22" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="2" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="2" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1847,92 +1920,71 @@
     <xf numFmtId="176" fontId="21" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="23" fillId="39" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="22" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="22" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="23" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="22" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="22" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="17" fillId="0" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="17" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="17" fillId="0" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="17" fillId="0" borderId="37" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="22" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="22" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="17" fillId="0" borderId="38" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="22" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="23" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="17" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="17" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="23" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="2" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="2" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="22" fillId="7" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="22" fillId="6" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="22" fillId="4" borderId="26" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="17" fillId="0" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="46">
@@ -2264,8 +2316,8 @@
   </sheetPr>
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8:M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -2273,11 +2325,11 @@
     <col min="1" max="1" width="18.453125" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.453125" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.08984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.08984375" style="1" customWidth="1"/>
     <col min="6" max="6" width="13" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.36328125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" style="1" customWidth="1"/>
     <col min="10" max="10" width="15.7265625" style="1" customWidth="1"/>
     <col min="11" max="11" width="13.90625" style="1" customWidth="1"/>
@@ -3361,401 +3413,399 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21.5" x14ac:dyDescent="0.4">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="5" t="s">
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="G2" s="5"/>
-      <c r="K2" s="7"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="G2" s="2"/>
+      <c r="K2" s="4"/>
       <c r="M2" s="1" t="str">
         <f ca="1">CONCATENATE("Update:",TEXT(O2,"[$-zh-TW]e/mm;@"))</f>
         <v>Update:112/09</v>
       </c>
-      <c r="O2" s="45">
+      <c r="O2" s="37">
         <f ca="1">TODAY()-31</f>
-        <v>45172</v>
+        <v>45174</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="82" t="s">
+      <c r="C3" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="82" t="s">
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="83"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="84"/>
-      <c r="N3" s="8" t="s">
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="9"/>
+      <c r="O3" s="6"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A4" s="77"/>
-      <c r="B4" s="80"/>
-      <c r="C4" s="85" t="s">
+      <c r="A4" s="57"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="74" t="s">
+      <c r="D4" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="74" t="s">
+      <c r="E4" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="66" t="s">
+      <c r="F4" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="72" t="s">
+      <c r="G4" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="73"/>
-      <c r="I4" s="71" t="s">
+      <c r="H4" s="51"/>
+      <c r="I4" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="72"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="74" t="s">
+      <c r="J4" s="50"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="66" t="s">
+      <c r="M4" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="57" t="str">
+      <c r="N4" s="67" t="str">
         <f ca="1">CONCATENATE("至",TEXT(O2,"[$-zh-TW]e/mm;@"))</f>
         <v>至112/09</v>
       </c>
-      <c r="O4" s="52" t="s">
+      <c r="O4" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="53"/>
-      <c r="Q4" s="30"/>
+      <c r="P4" s="77"/>
+      <c r="Q4" s="27"/>
     </row>
     <row r="5" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="78"/>
-      <c r="B5" s="81"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="10" t="s">
+      <c r="A5" s="58"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="K5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="75"/>
-      <c r="M5" s="67"/>
-      <c r="N5" s="58" t="str">
+      <c r="L5" s="49"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="68" t="str">
         <f t="shared" ref="N5" si="0">CONCATENATE("Update:",TEXT(P5,"[$-zh-TW]e/mm;@"))</f>
         <v>Update:1900/01</v>
       </c>
-      <c r="O5" s="12" t="s">
+      <c r="O5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="31"/>
+      <c r="P5" s="28"/>
     </row>
-    <row r="6" spans="1:17" s="32" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="34" t="s">
+    <row r="6" spans="1:17" s="29" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="35">
+      <c r="B6" s="79">
         <f>P4/1000000</f>
         <v>0</v>
       </c>
-      <c r="C6" s="36">
+      <c r="C6" s="80">
         <f>(E12+E13)/1000000</f>
         <v>0</v>
       </c>
-      <c r="D6" s="56">
+      <c r="D6" s="81">
         <f>(E8+E10)/1000000</f>
         <v>0</v>
       </c>
-      <c r="E6" s="13" t="e">
+      <c r="E6" s="82" t="e">
         <f>D6/C6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F6" s="37" t="e">
+      <c r="F6" s="83" t="e">
         <f>(E8+E10)/P4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G6" s="38">
+      <c r="G6" s="92">
         <f>I13/1000000</f>
         <v>0</v>
       </c>
-      <c r="H6" s="39">
+      <c r="H6" s="32">
         <f>((I12+L12)/1000000)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="39">
+      <c r="I6" s="32">
         <f>(I8+I10)/1000000</f>
         <v>0</v>
       </c>
-      <c r="J6" s="39">
+      <c r="J6" s="32">
         <v>0</v>
       </c>
-      <c r="K6" s="39">
+      <c r="K6" s="32">
         <f>L8/1000000</f>
         <v>0</v>
       </c>
-      <c r="L6" s="13" t="e">
+      <c r="L6" s="10" t="e">
         <f>(I6+J6+K6)/(G6+H6)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M6" s="37" t="e">
+      <c r="M6" s="31" t="e">
         <f>(I8+I10+L8)/P4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N6" s="40">
+      <c r="N6" s="33">
         <f>P5/1000000</f>
         <v>0</v>
       </c>
-      <c r="O6" s="24" t="s">
+      <c r="O6" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="P6" s="25"/>
+      <c r="P6" s="22"/>
     </row>
-    <row r="7" spans="1:17" s="32" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="69" t="s">
+    <row r="7" spans="1:17" s="29" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="44"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="43"/>
-      <c r="N7" s="44"/>
-      <c r="O7" s="59" t="s">
+      <c r="B7" s="89"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="90"/>
+      <c r="H7" s="91"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
+      <c r="L7" s="87"/>
+      <c r="M7" s="87"/>
+      <c r="N7" s="36"/>
+      <c r="O7" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="P7" s="60"/>
+      <c r="P7" s="70"/>
     </row>
-    <row r="8" spans="1:17" s="25" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="19"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="28" t="s">
+    <row r="8" spans="1:17" s="22" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="16"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="89"/>
-      <c r="F8" s="89"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="29" t="s">
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="87"/>
-      <c r="J8" s="87"/>
-      <c r="K8" s="41" t="s">
+      <c r="I8" s="84"/>
+      <c r="J8" s="84"/>
+      <c r="K8" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="L8" s="61"/>
-      <c r="M8" s="61"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="14" t="s">
+      <c r="L8" s="85"/>
+      <c r="M8" s="85"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="P8" s="26"/>
+      <c r="P8" s="23"/>
     </row>
-    <row r="9" spans="1:17" s="25" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="19"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="47" t="s">
+    <row r="9" spans="1:17" s="22" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="88"/>
-      <c r="F9" s="88"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="48" t="s">
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="62"/>
-      <c r="J9" s="62"/>
-      <c r="K9" s="49" t="s">
+      <c r="I9" s="74"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="L9" s="70"/>
-      <c r="M9" s="70"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="14" t="s">
+      <c r="L9" s="75"/>
+      <c r="M9" s="75"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="P9" s="26"/>
+      <c r="P9" s="23"/>
     </row>
-    <row r="10" spans="1:17" s="25" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="19"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="28" t="s">
+    <row r="10" spans="1:17" s="22" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="68"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="29" t="s">
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="63"/>
-      <c r="J10" s="63"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="24" t="s">
+      <c r="I10" s="74"/>
+      <c r="J10" s="74"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="P10" s="54"/>
+      <c r="P10" s="45"/>
     </row>
-    <row r="11" spans="1:17" s="25" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="19"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="47" t="s">
+    <row r="11" spans="1:17" s="22" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="16"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="48" t="s">
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="I11" s="62"/>
-      <c r="J11" s="62"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="24"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="74"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="21"/>
     </row>
-    <row r="12" spans="1:17" s="25" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="19"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21" t="s">
+    <row r="12" spans="1:17" s="22" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="16"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="65"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="50" t="s">
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="I12" s="64"/>
-      <c r="J12" s="64"/>
-      <c r="K12" s="51" t="s">
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="L12" s="64"/>
-      <c r="M12" s="64"/>
-      <c r="N12" s="24"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="21"/>
     </row>
     <row r="13" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="27"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="51" t="s">
+      <c r="A13" s="24"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="65"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="51" t="s">
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="I13" s="64"/>
-      <c r="J13" s="64"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="18"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="15"/>
     </row>
     <row r="14" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="27"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="18"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="15"/>
     </row>
     <row r="15" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="27"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="55" t="s">
+      <c r="A15" s="24"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="55" t="s">
+      <c r="E15" s="13"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="55" t="s">
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="L15" s="55"/>
-      <c r="M15" s="42"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="35"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="B16" s="7"/>
+      <c r="B16" s="4"/>
     </row>
     <row r="17" spans="15:15" x14ac:dyDescent="0.4">
-      <c r="O17" s="33"/>
+      <c r="O17" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I10:J10"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="L12:M12"/>
     <mergeCell ref="E13:F13"/>
@@ -3772,12 +3822,14 @@
     <mergeCell ref="G3:M3"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="E12:F12"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E8:F8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.39370078740157483" bottom="0.39370078740157483" header="0.51181102362204722" footer="5.1181102362204731"/>

</xml_diff>